<commit_message>
I have modificated profile
</commit_message>
<xml_diff>
--- a/public/foldercompanies/LlakaScript/LlakaScript.xlsx
+++ b/public/foldercompanies/LlakaScript/LlakaScript.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="27">
   <si>
     <t xml:space="preserve">Menu_Title</t>
   </si>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Pizza</t>
   </si>
   <si>
-    <t xml:space="preserve">profile_one</t>
+    <t xml:space="preserve">profile_ten</t>
   </si>
   <si>
     <t xml:space="preserve">#33ffff</t>
@@ -70,28 +70,34 @@
     <t xml:space="preserve">#d2a700</t>
   </si>
   <si>
+    <t xml:space="preserve">fondo.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lasagna.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">primera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lasagna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asaña clásica con carne y salsa bechamel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cucina Italiana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">profile_three</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#9b1c31</t>
+  </si>
+  <si>
     <t xml:space="preserve">background-food.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lasagna.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">primera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lasagna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asaña clásica con carne y salsa bechamel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cucina Italiana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#9b1c31</t>
   </si>
   <si>
     <t xml:space="preserve">segunda</t>
@@ -241,10 +247,10 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B21"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.85"/>
@@ -339,16 +345,16 @@
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>17</v>
@@ -377,16 +383,16 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>17</v>
@@ -415,22 +421,22 @@
         <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H5" s="3" t="n">
         <v>1</v>
@@ -453,22 +459,22 @@
         <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H6" s="4" t="n">
         <v>1</v>
@@ -491,7 +497,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>14</v>
@@ -500,7 +506,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>17</v>
@@ -529,16 +535,16 @@
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>17</v>
@@ -567,16 +573,16 @@
         <v>22</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>17</v>
@@ -605,22 +611,22 @@
         <v>22</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H10" s="3" t="n">
         <v>1</v>
@@ -643,22 +649,22 @@
         <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H11" s="4" t="n">
         <v>1</v>
@@ -681,7 +687,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>14</v>
@@ -690,7 +696,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>17</v>
@@ -719,16 +725,16 @@
         <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>17</v>
@@ -757,16 +763,16 @@
         <v>22</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>17</v>
@@ -795,22 +801,22 @@
         <v>22</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H15" s="3" t="n">
         <v>1</v>
@@ -833,22 +839,22 @@
         <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H16" s="4" t="n">
         <v>1</v>
@@ -871,7 +877,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>14</v>
@@ -879,8 +885,8 @@
       <c r="D17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>16</v>
+      <c r="E17" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>17</v>
@@ -909,16 +915,16 @@
         <v>22</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>16</v>
+      <c r="E18" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>17</v>
@@ -947,16 +953,16 @@
         <v>22</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>16</v>
+      <c r="E19" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>17</v>
@@ -985,22 +991,22 @@
         <v>22</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>16</v>
+      <c r="E20" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H20" s="4" t="n">
         <v>1</v>
@@ -1023,22 +1029,22 @@
         <v>22</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>16</v>
+      <c r="E21" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H21" s="4" t="n">
         <v>1</v>

</xml_diff>